<commit_message>
Updated persona task overview
</commit_message>
<xml_diff>
--- a/docs/PersonaTaskOverview.xlsx
+++ b/docs/PersonaTaskOverview.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Gurli-Margrethe</t>
   </si>
@@ -28,15 +28,6 @@
   </si>
   <si>
     <t>Jason</t>
-  </si>
-  <si>
-    <t>Clerks</t>
-  </si>
-  <si>
-    <t>Managers</t>
-  </si>
-  <si>
-    <t>The Board</t>
   </si>
   <si>
     <r>
@@ -125,6 +116,18 @@
   </si>
   <si>
     <t>Check reservation</t>
+  </si>
+  <si>
+    <t>View current lane schedule for a given day</t>
+  </si>
+  <si>
+    <t>Adonis</t>
+  </si>
+  <si>
+    <t>Pythagoras</t>
+  </si>
+  <si>
+    <t>Jørgen</t>
   </si>
 </sst>
 </file>
@@ -502,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,213 +535,221 @@
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added manager task of setting up lanes and timeslots in the system
</commit_message>
<xml_diff>
--- a/docs/PersonaTaskOverview.xlsx
+++ b/docs/PersonaTaskOverview.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Gurli-Margrethe</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Jørgen</t>
+  </si>
+  <si>
+    <t>Setup Lanes and TimeSlots</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,6 +688,11 @@
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>